<commit_message>
Camss sis technical requirements was added to the document
</commit_message>
<xml_diff>
--- a/SIS/doc/functional_&_technical_specifications/srs_system_requirements_specifications_CAMSS_SIS.xlsx
+++ b/SIS/doc/functional_&_technical_specifications/srs_system_requirements_specifications_CAMSS_SIS.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SEMBU\Github\CAMSS\CAMSS_as_a_Hub\SIS\doc\functional_&amp;_technical_specifications\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SEMBU\Github\CAMSS\CAMSS_Hub\SIS\doc\functional_&amp;_technical_specifications\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ABAD4F2-EF96-4D0E-BD02-48666C1930BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A289116A-CCD0-4DCA-AD58-2E3377AB60D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-972" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{38C542F3-FE27-4179-B574-1C96884F70A0}"/>
+    <workbookView xWindow="22932" yWindow="-972" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{38C542F3-FE27-4179-B574-1C96884F70A0}"/>
   </bookViews>
   <sheets>
     <sheet name="SCOPE" sheetId="1" r:id="rId1"/>
@@ -35,8 +35,26 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={78B52DA1-F906-419C-A4D1-962BDB52E5DD}</author>
+  </authors>
+  <commentList>
+    <comment ref="D7" authorId="0" shapeId="0" xr:uid="{78B52DA1-F906-419C-A4D1-962BDB52E5DD}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Is it missing?</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="219">
   <si>
     <t>USE CASE</t>
   </si>
@@ -95,16 +113,10 @@
     <t>3.3.4.3.Model Training and Testing</t>
   </si>
   <si>
-    <t>3.3.1.3. Terms Frecuency</t>
-  </si>
-  <si>
     <t>3.3.1.2. Named Entity Recognition NER</t>
   </si>
   <si>
     <t>3.3.2. Lemmatize Corpora</t>
-  </si>
-  <si>
-    <t>3.3.3. Resource relevance</t>
   </si>
   <si>
     <t>3.3.4. Historification</t>
@@ -191,12 +203,6 @@
   </si>
   <si>
     <t>Capture concepts from the resource content in order to compare the extracted concepts to similar or identical concepts maintained in one or more Thesauri, database, index tables, etc.</t>
-  </si>
-  <si>
-    <t>Calculation of the probability that a given resource is or not an interoperability specification of a certain type.</t>
-  </si>
-  <si>
-    <t>Help the user to determinate wether a resource can be judged an interoperability specification.</t>
   </si>
   <si>
     <t>Save the results of the corpora analysis in a storage system.</t>
@@ -394,11 +400,6 @@
     <t>RATIONALE</t>
   </si>
   <si>
-    <t>* Backwards compatibility with previous CAMSS developments
-* Take leverage of logic inference
-* Aligment to other existing developments in the contexts of DEP such as EIRA</t>
-  </si>
-  <si>
     <t>ID</t>
   </si>
   <si>
@@ -473,10 +474,6 @@
     <t>RELATED REQUIREMENTS</t>
   </si>
   <si>
-    <t>DR-1
-DR-2</t>
-  </si>
-  <si>
     <t>This task entails reusing an existing lemmatiser and an ad hoc development of configuration</t>
   </si>
   <si>
@@ -508,10 +505,6 @@
     <t>CAMSS SIS  source code development</t>
   </si>
   <si>
-    <t xml:space="preserve">IR-3
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">IR-4
 </t>
   </si>
@@ -541,9 +534,6 @@
     <t>F3-3-1-3</t>
   </si>
   <si>
-    <t>F3-3-3</t>
-  </si>
-  <si>
     <t>F3-3-4</t>
   </si>
   <si>
@@ -623,13 +613,155 @@
   </si>
   <si>
     <t>1.</t>
+  </si>
+  <si>
+    <t>* Backwards compatibility with previous CAMSS developments.
+* Take leverage of logic inference
+* Aligment to other existing developments in the contexts of DEP such as EIRA</t>
+  </si>
+  <si>
+    <t>IR-6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IR-5
+</t>
+  </si>
+  <si>
+    <t>* For the lemmatisation to be correct the lenguage need to be detected</t>
+  </si>
+  <si>
+    <t>IR-3, IR-4</t>
+  </si>
+  <si>
+    <t>IR-7</t>
+  </si>
+  <si>
+    <t>DR-3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Team SHOULD define the method of Linking &amp; Indexation of lemmas between Thesauri and Corpora </t>
+  </si>
+  <si>
+    <t>El sistema DEBERÁ utilizar el método de Linking &amp; Indexation dependiendo del tamaño del Thesauri y el Corpora</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* El orden en que se ejecute el método de Linking &amp; Indexation dependerá del tamaño del Thesauri y el Corpora.
+e.g. Thesari 500 lemmas, Corpora 50 docs with 1000 lemmas de media cada doc
+ - Thesariu vs Corpora: Para cada lemma del thesauri se busca en cada documento del Corpora. Iteraciones: 500x50
+ - Corpora vs Thesauri: Para cada lemma de cada documento se busca en la taxonomia. Iteraciones: 1000x50
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* CAMSS SIS needs to specify which method to implement of Linking &amp; Indexation because it impacts in the processing time.
+</t>
+  </si>
+  <si>
+    <t>DR-3
+IR-7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IR-8 </t>
+  </si>
+  <si>
+    <t>El sistema DEBERÁ consumir una API para descargar los recursos que conforman Corpora</t>
+  </si>
+  <si>
+    <t>* Es importante realizar la descarga de los recursos mediante una API y así evitar las depedencias con una UI</t>
+  </si>
+  <si>
+    <t>IR-8</t>
+  </si>
+  <si>
+    <t>DR-4</t>
+  </si>
+  <si>
+    <t>The system MUST textify only the documents with the desired extensions.</t>
+  </si>
+  <si>
+    <t>* Sólo se considerarán los documentos que sean descriptivos que tengan texto plano
+* las extensiones de interés compatibles con la textificación son: .txt, .pdf, .doc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IR-9 </t>
+  </si>
+  <si>
+    <t>IR-9</t>
+  </si>
+  <si>
+    <t>IR-10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           3.3.1.3. Terms Frecuency as minimal relevance indicator</t>
+  </si>
+  <si>
+    <t>The max length of the concepts MUST be identified</t>
+  </si>
+  <si>
+    <t>The system MUST calculate the number of the occurrences of the n-grams in a resource.</t>
+  </si>
+  <si>
+    <t>* El cálculo de las ocurrencias es importante para ordenar los recurosos por relevancia.</t>
+  </si>
+  <si>
+    <t>* The max length es necesario para definir el n-gram 
+* A su vez el n-gram permite identificar los conceptos que se definen con n palabras</t>
+  </si>
+  <si>
+    <t>IR-11</t>
+  </si>
+  <si>
+    <t>Each n-gram of the Corpora resource MUST be lemmatised.</t>
+  </si>
+  <si>
+    <t>Corpora maintenance</t>
+  </si>
+  <si>
+    <t>IR-12</t>
+  </si>
+  <si>
+    <t>Each n-gram language MUST be identified</t>
+  </si>
+  <si>
+    <t>Each label language MUST be identified</t>
+  </si>
+  <si>
+    <t>DR-1
+IR-3</t>
+  </si>
+  <si>
+    <t>DR-1
+IR-11</t>
+  </si>
+  <si>
+    <t>IR-11 y IR-12</t>
+  </si>
+  <si>
+    <t>IR-13</t>
+  </si>
+  <si>
+    <t>The n-grams lemmas of the Corpora resourse MUST be saved in a database</t>
+  </si>
+  <si>
+    <t>* Is important to persist the results of the analysis to avoid loss of performance and unnecessary operations. Ensure business continuity in the mid and long term.</t>
+  </si>
+  <si>
+    <t>DR-5</t>
+  </si>
+  <si>
+    <t>A datamodel MUST be defined to preserve the lemmatised Corpora</t>
+  </si>
+  <si>
+    <t>* Son importante para describir las estructuras de datos y permitir la manipulación de los mismos.</t>
+  </si>
+  <si>
+    <t>All activities related to store and preserve the analysis results</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -658,6 +790,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="15">
@@ -746,7 +884,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -800,26 +938,6 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -919,6 +1037,18 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -929,52 +1059,36 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1000,6 +1114,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Manuela Grajales Duque" id="{D24AAA2D-0A9B-471F-9458-CDCF7779D6F5}" userId="Manuela Grajales Duque" providerId="None"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1297,50 +1417,61 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="D7" dT="2021-12-15T11:42:53.09" personId="{D24AAA2D-0A9B-471F-9458-CDCF7779D6F5}" id="{78B52DA1-F906-419C-A4D1-962BDB52E5DD}">
+    <text>Is it missing?</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB53E975-4778-42ED-88A6-825C9DDA12C7}">
-  <dimension ref="A1:J28"/>
+  <dimension ref="A1:K28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView topLeftCell="F7" workbookViewId="0">
+      <selection activeCell="F18" sqref="A18:XFD18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="5" width="2.81640625" style="7" customWidth="1"/>
+    <col min="1" max="5" width="2.81640625" style="7" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="53.26953125" style="7" customWidth="1"/>
-    <col min="7" max="7" width="19.7265625" style="7" customWidth="1"/>
-    <col min="8" max="9" width="31.1796875" style="7" customWidth="1"/>
-    <col min="10" max="10" width="29" style="7" customWidth="1"/>
-    <col min="11" max="16384" width="8.7265625" style="7"/>
+    <col min="7" max="8" width="19.7265625" style="7" customWidth="1"/>
+    <col min="9" max="9" width="31.1796875" style="7" customWidth="1"/>
+    <col min="10" max="10" width="76.81640625" style="7" customWidth="1"/>
+    <col min="11" max="11" width="29" style="7" customWidth="1"/>
+    <col min="12" max="16384" width="8.7265625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="F1" s="32" t="s">
-        <v>81</v>
-      </c>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F1" s="36" t="s">
+        <v>77</v>
+      </c>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="F2" s="8" t="s">
         <v>0</v>
       </c>
       <c r="G2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="H2" s="8"/>
+      <c r="I2" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="7">
         <v>1</v>
       </c>
@@ -1354,8 +1485,9 @@
       <c r="G3" s="10"/>
       <c r="H3" s="10"/>
       <c r="I3" s="10"/>
-    </row>
-    <row r="4" spans="1:10" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="J3" s="10"/>
+    </row>
+    <row r="4" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A4" s="7">
         <v>2</v>
       </c>
@@ -1369,18 +1501,18 @@
       <c r="G4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="7" t="str">
-        <f>'TECHNICAL REQUIREMENT'!A11</f>
+      <c r="I4" s="7" t="str">
+        <f>'TECHNICAL REQUIREMENT'!A15</f>
         <v>IR-2</v>
       </c>
-      <c r="I4" s="7" t="s">
-        <v>125</v>
-      </c>
       <c r="J4" s="7" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+        <v>120</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A5" s="7">
         <v>3</v>
       </c>
@@ -1394,18 +1526,21 @@
       <c r="G5" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="H5" s="7" t="str">
-        <f>'TECHNICAL REQUIREMENT'!A12</f>
-        <v xml:space="preserve">IR-3 </v>
-      </c>
-      <c r="I5" s="7" t="s">
-        <v>136</v>
+      <c r="H5" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="I5" s="7" t="str">
+        <f>'TECHNICAL REQUIREMENT'!A17</f>
+        <v>IR-4</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+        <v>130</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="7">
         <v>4</v>
       </c>
@@ -1419,18 +1554,18 @@
       <c r="G6" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="H6" s="49" t="str">
-        <f>_xlfn.CONCAT('TECHNICAL REQUIREMENT'!A13, ", ", 'TECHNICAL REQUIREMENT'!A14)</f>
-        <v>IR-4, IR-5</v>
-      </c>
-      <c r="I6" s="7" t="s">
-        <v>148</v>
+      <c r="I6" s="34" t="str">
+        <f>_xlfn.CONCAT('TECHNICAL REQUIREMENT'!A18, ", ", 'TECHNICAL REQUIREMENT'!A19)</f>
+        <v>IR-5, IR-6</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+        <v>141</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="7">
         <v>5</v>
       </c>
@@ -1441,11 +1576,16 @@
       <c r="F7" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
+      <c r="G7" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="H7" s="10" t="s">
+        <v>187</v>
+      </c>
       <c r="I7" s="10"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="J7" s="10"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="7">
         <v>6</v>
       </c>
@@ -1459,8 +1599,9 @@
       <c r="G8" s="10"/>
       <c r="H8" s="10"/>
       <c r="I8" s="10"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="J8" s="10"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="7">
         <v>7</v>
       </c>
@@ -1470,24 +1611,33 @@
       <c r="G9" s="7" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="H9" s="7" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="F10" s="25" t="s">
         <v>11</v>
       </c>
       <c r="G10" s="7" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="H10" s="7" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="F11" s="25" t="s">
         <v>12</v>
       </c>
       <c r="G11" s="7" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="H11" s="7" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="F12" s="26" t="s">
         <v>14</v>
       </c>
@@ -1496,8 +1646,9 @@
       </c>
       <c r="H12" s="24"/>
       <c r="I12" s="24"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="J12" s="24"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="F13" s="28" t="s">
         <v>15</v>
       </c>
@@ -1505,52 +1656,62 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="F14" s="28" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G14" s="7" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="174" x14ac:dyDescent="0.35">
-      <c r="F15" s="28" t="s">
-        <v>150</v>
-      </c>
-      <c r="G15" s="7" t="s">
+    <row r="15" spans="1:11" s="46" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="F15" s="47" t="s">
+        <v>198</v>
+      </c>
+      <c r="G15" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="I15" s="29" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="H15" s="46" t="s">
+        <v>197</v>
+      </c>
+      <c r="J15" s="48" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="F16" s="27" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G16" s="7" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="17" spans="6:10" x14ac:dyDescent="0.35">
+      <c r="H16" s="7" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="17" spans="6:11" x14ac:dyDescent="0.35">
       <c r="F17" s="26" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G17" s="24" t="s">
         <v>3</v>
       </c>
       <c r="H17" s="24"/>
       <c r="I17" s="24"/>
-    </row>
-    <row r="18" spans="6:10" x14ac:dyDescent="0.35">
+      <c r="J17" s="24"/>
+    </row>
+    <row r="18" spans="6:11" x14ac:dyDescent="0.35">
       <c r="F18" s="28" t="s">
         <v>16</v>
       </c>
       <c r="G18" s="7" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="19" spans="6:10" x14ac:dyDescent="0.35">
+      <c r="H18" s="7" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="19" spans="6:11" x14ac:dyDescent="0.35">
       <c r="F19" s="28" t="s">
         <v>17</v>
       </c>
@@ -1558,7 +1719,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="6:10" x14ac:dyDescent="0.35">
+    <row r="20" spans="6:11" x14ac:dyDescent="0.35">
       <c r="F20" s="28" t="s">
         <v>18</v>
       </c>
@@ -1566,7 +1727,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="6:10" x14ac:dyDescent="0.35">
+    <row r="21" spans="6:11" x14ac:dyDescent="0.35">
       <c r="F21" s="25" t="s">
         <v>13</v>
       </c>
@@ -1574,88 +1735,93 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="6:10" x14ac:dyDescent="0.35">
+    <row r="22" spans="6:11" x14ac:dyDescent="0.35">
       <c r="F22" s="10" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="G22" s="10" t="s">
         <v>3</v>
       </c>
       <c r="H22" s="10"/>
       <c r="I22" s="10"/>
-    </row>
-    <row r="23" spans="6:10" x14ac:dyDescent="0.35">
+      <c r="J22" s="10"/>
+    </row>
+    <row r="23" spans="6:11" x14ac:dyDescent="0.35">
       <c r="F23" s="10" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="G23" s="10"/>
       <c r="H23" s="10"/>
       <c r="I23" s="10"/>
-    </row>
-    <row r="24" spans="6:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="J23" s="10"/>
+    </row>
+    <row r="24" spans="6:11" x14ac:dyDescent="0.35">
       <c r="F24" s="25" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="G24" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="I24" s="7" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="25" spans="6:10" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="J24" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="25" spans="6:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="F25" s="25" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="G25" s="29" t="s">
         <v>2</v>
       </c>
       <c r="H25" s="29"/>
-      <c r="I25" s="29" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="26" spans="6:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="I25" s="29"/>
+      <c r="J25" s="29" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="26" spans="6:11" ht="29" x14ac:dyDescent="0.35">
       <c r="F26" s="25" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="G26" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="I26" s="7" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="27" spans="6:10" ht="116" x14ac:dyDescent="0.35">
+      <c r="J26" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="27" spans="6:11" ht="116" x14ac:dyDescent="0.35">
       <c r="F27" s="10" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="G27" s="10" t="s">
         <v>3</v>
       </c>
       <c r="H27" s="10"/>
-      <c r="I27" s="31" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="28" spans="6:10" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="I27" s="10"/>
+      <c r="J27" s="31" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="28" spans="6:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="F28" s="10" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="G28" s="10" t="s">
         <v>3</v>
       </c>
       <c r="H28" s="10"/>
-      <c r="I28" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="J28" s="31" t="s">
-        <v>105</v>
+      <c r="I28" s="10"/>
+      <c r="J28" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="K28" s="31" t="s">
+        <v>101</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="F1:J1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1663,17 +1829,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E5040CC-E52B-4256-BF51-9E73A75A719C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E5040CC-E52B-4256-BF51-9E73A75A719C}">
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:B6"/>
+    <sheetView topLeftCell="C18" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.453125" style="50" customWidth="1"/>
-    <col min="2" max="2" width="19.36328125" style="6" customWidth="1"/>
+    <col min="1" max="1" width="10.453125" style="35" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="19.36328125" style="6" hidden="1" customWidth="1"/>
     <col min="3" max="3" width="20.453125" style="1" customWidth="1"/>
     <col min="4" max="6" width="20.453125" style="2" customWidth="1"/>
     <col min="7" max="8" width="50.26953125" style="5" customWidth="1"/>
@@ -1682,157 +1848,150 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="31" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C1" s="33" t="s">
-        <v>80</v>
-      </c>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
+      <c r="C1" s="37" t="s">
+        <v>76</v>
+      </c>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C2" s="12" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="G2" s="11" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H2" s="11" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="58" x14ac:dyDescent="0.35">
-      <c r="A3" s="50" t="s">
-        <v>183</v>
+      <c r="A3" s="35" t="s">
+        <v>175</v>
       </c>
       <c r="B3" s="6" t="str">
         <f>_xlfn.CONCAT(A3, " ", C3)</f>
         <v>1. Thesauri Concepts Processing</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="58" x14ac:dyDescent="0.35">
-      <c r="A4" s="50" t="s">
-        <v>173</v>
+      <c r="A4" s="35" t="s">
+        <v>165</v>
       </c>
       <c r="B4" s="6" t="str">
         <f>_xlfn.CONCAT(A4, " ", D4)</f>
         <v>1.1 Thesauri Concepts Edition and Maintenance</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="I4" s="1"/>
     </row>
     <row r="5" spans="1:9" ht="58" x14ac:dyDescent="0.35">
-      <c r="A5" s="50" t="s">
-        <v>174</v>
+      <c r="A5" s="35" t="s">
+        <v>166</v>
       </c>
       <c r="B5" s="6" t="str">
         <f t="shared" ref="B5:B6" si="0">_xlfn.CONCAT(A5, " ", D5)</f>
         <v>1.2 Thesauri Concepts Lemmatization</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="I5" s="1"/>
     </row>
     <row r="6" spans="1:9" ht="60.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="50" t="s">
-        <v>175</v>
+      <c r="A6" s="35" t="s">
+        <v>167</v>
       </c>
       <c r="B6" s="6" t="str">
         <f t="shared" si="0"/>
         <v>1.3  Thesauri Exportation and Loading</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="G6" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="1:9" ht="60.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D7" s="49" t="s">
+        <v>21</v>
+      </c>
+      <c r="I7" s="1"/>
+    </row>
+    <row r="8" spans="1:9" ht="87.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="35" t="s">
+        <v>168</v>
+      </c>
+      <c r="B8" s="6" t="str">
+        <f>_xlfn.CONCAT(A8, ". ", C8)</f>
+        <v>2. Keyterm-Resource Linking &amp; Indexation</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="D8" s="15"/>
+      <c r="G8" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H8" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="H6" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="I6" s="1"/>
-    </row>
-    <row r="7" spans="1:9" ht="87.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="50" t="s">
-        <v>176</v>
-      </c>
-      <c r="B7" s="6" t="str">
-        <f>_xlfn.CONCAT(A7, ". ", C7)</f>
-        <v>2. Keyterm-Resource Linking &amp; Indexation</v>
-      </c>
-      <c r="C7" s="14" t="s">
-        <v>177</v>
-      </c>
-      <c r="D7" s="15"/>
-      <c r="G7" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" s="7" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="50"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="4" t="str">
+      <c r="I8" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" s="7" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="35"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="4" t="str">
         <f>F21</f>
         <v>3.3.4.1. Store and preserve the analysis results</v>
-      </c>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="16"/>
-    </row>
-    <row r="9" spans="1:9" s="7" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A9" s="50"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="4" t="str">
-        <f>D24</f>
-        <v>3.4. Metadata Preservation</v>
       </c>
       <c r="E9" s="15"/>
       <c r="F9" s="15"/>
@@ -1840,74 +1999,72 @@
       <c r="H9" s="18"/>
       <c r="I9" s="16"/>
     </row>
-    <row r="10" spans="1:9" ht="58" x14ac:dyDescent="0.35">
-      <c r="A10" s="50" t="s">
-        <v>178</v>
-      </c>
-      <c r="C10" s="17" t="s">
+    <row r="10" spans="1:9" s="7" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A10" s="35"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="4" t="str">
+        <f>D24</f>
+        <v>3.4. Metadata Preservation</v>
+      </c>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="16"/>
+    </row>
+    <row r="11" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+      <c r="A11" s="35" t="s">
+        <v>170</v>
+      </c>
+      <c r="C11" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="G10" s="5" t="s">
+      <c r="G11" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A12" s="35" t="s">
+        <v>171</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="H10" s="5" t="s">
+      <c r="H12" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="I10" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A11" s="50" t="s">
-        <v>179</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G11" s="5" t="s">
+      <c r="I12" s="1"/>
+    </row>
+    <row r="13" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A13" s="35" t="s">
+        <v>172</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G13" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="H11" s="5" t="s">
+      <c r="H13" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="I11" s="1"/>
-    </row>
-    <row r="12" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A12" s="50" t="s">
-        <v>180</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G12" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="H12" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="I12" s="1"/>
-    </row>
-    <row r="13" spans="1:9" ht="87" x14ac:dyDescent="0.35">
-      <c r="A13" s="50" t="s">
-        <v>181</v>
-      </c>
-      <c r="D13" s="4" t="s">
+      <c r="I13" s="1"/>
+    </row>
+    <row r="14" spans="1:9" ht="87" x14ac:dyDescent="0.35">
+      <c r="A14" s="35" t="s">
+        <v>173</v>
+      </c>
+      <c r="D14" s="4" t="s">
         <v>12</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="H13" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="I13" s="1"/>
-    </row>
-    <row r="14" spans="1:9" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="50" t="s">
-        <v>152</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>14</v>
       </c>
       <c r="G14" s="5" t="s">
         <v>44</v>
@@ -1917,267 +2074,267 @@
       </c>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A15" s="50" t="s">
-        <v>182</v>
-      </c>
-      <c r="F15" s="4" t="s">
+    <row r="15" spans="1:9" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="35" t="s">
+        <v>145</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="I15" s="1"/>
+    </row>
+    <row r="16" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A16" s="35" t="s">
+        <v>174</v>
+      </c>
+      <c r="F16" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G15" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="H15" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="I15" s="1"/>
-    </row>
-    <row r="16" spans="1:9" ht="87" x14ac:dyDescent="0.35">
-      <c r="A16" s="50" t="s">
-        <v>154</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>20</v>
-      </c>
       <c r="G16" s="5" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="50" t="s">
-        <v>155</v>
+    <row r="17" spans="1:9" ht="87" x14ac:dyDescent="0.35">
+      <c r="A17" s="35" t="s">
+        <v>147</v>
       </c>
       <c r="F17" s="4" t="s">
         <v>19</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="1:9" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="50" t="s">
-        <v>153</v>
-      </c>
-      <c r="E18" s="4" t="s">
+    <row r="18" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A18" s="35" t="s">
+        <v>148</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="H18" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="I18" s="1"/>
+    </row>
+    <row r="19" spans="1:9" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="35" t="s">
+        <v>146</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="H19" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="I19" s="1"/>
+    </row>
+    <row r="20" spans="1:9" ht="87" x14ac:dyDescent="0.35">
+      <c r="A20" s="35" t="s">
+        <v>149</v>
+      </c>
+      <c r="E20" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G18" s="5" t="s">
+      <c r="G20" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="H18" s="5" t="s">
+      <c r="H20" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="I18" s="1"/>
-    </row>
-    <row r="19" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A19" s="50" t="s">
-        <v>156</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G19" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="H19" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="I19" s="1"/>
-    </row>
-    <row r="20" spans="1:9" ht="87" x14ac:dyDescent="0.35">
-      <c r="A20" s="50" t="s">
-        <v>157</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G20" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="H20" s="5" t="s">
-        <v>53</v>
-      </c>
       <c r="I20" s="1"/>
     </row>
     <row r="21" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A21" s="50" t="s">
-        <v>158</v>
+      <c r="A21" s="35" t="s">
+        <v>150</v>
       </c>
       <c r="F21" s="4" t="s">
         <v>16</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="I21" s="1"/>
     </row>
     <row r="22" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A22" s="50" t="s">
-        <v>159</v>
+      <c r="A22" s="35" t="s">
+        <v>151</v>
       </c>
       <c r="F22" s="4" t="s">
         <v>17</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="I22" s="1"/>
     </row>
     <row r="23" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A23" s="50" t="s">
-        <v>160</v>
+      <c r="A23" s="35" t="s">
+        <v>152</v>
       </c>
       <c r="F23" s="4" t="s">
         <v>18</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="I23" s="1"/>
     </row>
     <row r="24" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A24" s="50" t="s">
-        <v>161</v>
+      <c r="A24" s="35" t="s">
+        <v>153</v>
       </c>
       <c r="D24" s="4" t="s">
         <v>13</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I24" s="1"/>
     </row>
     <row r="25" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A25" s="50" t="s">
-        <v>162</v>
+      <c r="A25" s="35" t="s">
+        <v>154</v>
       </c>
       <c r="C25" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="H25" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+      <c r="A26" s="35" t="s">
+        <v>155</v>
+      </c>
+      <c r="C26" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="G26" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="H26" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="35" t="s">
+        <v>156</v>
+      </c>
+      <c r="D27" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="G25" s="5" t="s">
+      <c r="G27" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="H27" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="I27" s="1"/>
+    </row>
+    <row r="28" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A28" s="35" t="s">
+        <v>157</v>
+      </c>
+      <c r="D28" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="H25" s="5" t="s">
+      <c r="G28" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="H28" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="I28" s="1"/>
+    </row>
+    <row r="29" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A29" s="35" t="s">
+        <v>158</v>
+      </c>
+      <c r="D29" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="I25" s="1" t="s">
+      <c r="G29" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="H29" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="I29" s="1"/>
+    </row>
+    <row r="30" spans="1:9" ht="90" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="35" t="s">
+        <v>159</v>
+      </c>
+      <c r="C30" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="G30" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="H30" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="I30" s="30" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+      <c r="A31" s="35" t="s">
+        <v>160</v>
+      </c>
+      <c r="C31" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="H31" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="I31" s="30" t="s">
         <v>101</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" ht="58" x14ac:dyDescent="0.35">
-      <c r="A26" s="50" t="s">
-        <v>163</v>
-      </c>
-      <c r="C26" s="20" t="s">
-        <v>71</v>
-      </c>
-      <c r="G26" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="H26" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="I26" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="50" t="s">
-        <v>164</v>
-      </c>
-      <c r="D27" s="21" t="s">
-        <v>72</v>
-      </c>
-      <c r="G27" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="H27" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="I27" s="1"/>
-    </row>
-    <row r="28" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A28" s="50" t="s">
-        <v>165</v>
-      </c>
-      <c r="D28" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="G28" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="H28" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="I28" s="1"/>
-    </row>
-    <row r="29" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A29" s="50" t="s">
-        <v>166</v>
-      </c>
-      <c r="D29" s="21" t="s">
-        <v>74</v>
-      </c>
-      <c r="G29" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="H29" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="I29" s="1"/>
-    </row>
-    <row r="30" spans="1:9" ht="90" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="50" t="s">
-        <v>167</v>
-      </c>
-      <c r="C30" s="22" t="s">
-        <v>82</v>
-      </c>
-      <c r="G30" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="H30" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="I30" s="30" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" ht="58" x14ac:dyDescent="0.35">
-      <c r="A31" s="50" t="s">
-        <v>168</v>
-      </c>
-      <c r="C31" s="23" t="s">
-        <v>83</v>
-      </c>
-      <c r="G31" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="H31" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="I31" s="30" t="s">
-        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -2190,283 +2347,427 @@
   <ignoredErrors>
     <ignoredError sqref="A5 A4" numberStoredAsText="1"/>
   </ignoredErrors>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05B4DD8A-68C0-4698-9F66-34436918ED09}">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" style="36"/>
-    <col min="2" max="2" width="23.90625" style="36" customWidth="1"/>
-    <col min="3" max="3" width="46.36328125" style="36" customWidth="1"/>
-    <col min="4" max="4" width="32.6328125" style="36" customWidth="1"/>
-    <col min="5" max="5" width="22.90625" style="36" customWidth="1"/>
-    <col min="6" max="16384" width="8.7265625" style="36"/>
+    <col min="1" max="1" width="8.7265625" style="5"/>
+    <col min="2" max="2" width="23.90625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="46.36328125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="32.6328125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="22.90625" style="5" customWidth="1"/>
+    <col min="6" max="16384" width="8.7265625" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="38" t="s">
+        <v>109</v>
+      </c>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="39"/>
+    </row>
+    <row r="2" spans="1:5" ht="24.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B2" s="40"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41" t="s">
+        <v>74</v>
+      </c>
+      <c r="E2" s="42"/>
+    </row>
+    <row r="3" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="B3" s="43" t="s">
+        <v>105</v>
+      </c>
+      <c r="C3" s="44" t="s">
+        <v>106</v>
+      </c>
+      <c r="D3" s="44" t="s">
+        <v>103</v>
+      </c>
+      <c r="E3" s="45" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="B4" s="32" t="s">
+        <v>104</v>
+      </c>
+      <c r="C4" s="32" t="s">
+        <v>176</v>
+      </c>
+      <c r="D4" s="32" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="33"/>
+    </row>
+    <row r="5" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+      <c r="A5" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="B5" s="32" t="s">
+        <v>127</v>
+      </c>
+      <c r="C5" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="D5" s="32" t="s">
+        <v>128</v>
+      </c>
+      <c r="E5" s="33"/>
+    </row>
+    <row r="6" spans="1:5" ht="174" x14ac:dyDescent="0.35">
+      <c r="A6" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="B6" s="32" t="s">
+        <v>183</v>
+      </c>
+      <c r="C6" s="32" t="s">
+        <v>185</v>
+      </c>
+      <c r="D6" s="32" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="33"/>
+    </row>
+    <row r="7" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="C7" s="32" t="s">
+        <v>202</v>
+      </c>
+      <c r="D7" s="32" t="s">
+        <v>128</v>
+      </c>
+      <c r="E7" s="33"/>
+    </row>
+    <row r="8" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="B8" s="32" t="s">
+        <v>216</v>
+      </c>
+      <c r="C8" s="32" t="s">
+        <v>217</v>
+      </c>
+      <c r="D8" s="32" t="s">
+        <v>218</v>
+      </c>
+      <c r="E8" s="33"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B9" s="32"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="33"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B10" s="32"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="33"/>
+    </row>
+    <row r="11" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B11" s="32"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="33"/>
+    </row>
+    <row r="12" spans="1:5" ht="24.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B12" s="40"/>
+      <c r="C12" s="41"/>
+      <c r="D12" s="41" t="s">
+        <v>75</v>
+      </c>
+      <c r="E12" s="42"/>
+    </row>
+    <row r="13" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="B13" s="43" t="s">
+        <v>105</v>
+      </c>
+      <c r="C13" s="44" t="s">
+        <v>106</v>
+      </c>
+      <c r="D13" s="44" t="s">
         <v>114</v>
       </c>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="35"/>
-    </row>
-    <row r="2" spans="1:5" ht="24.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="37"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38" t="s">
-        <v>78</v>
-      </c>
-      <c r="E2" s="39"/>
-    </row>
-    <row r="3" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="36" t="s">
+      <c r="E13" s="45" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="116" x14ac:dyDescent="0.35">
+      <c r="A14" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B14" s="32" t="s">
         <v>112</v>
       </c>
-      <c r="B3" s="40" t="s">
-        <v>109</v>
-      </c>
-      <c r="C3" s="41" t="s">
+      <c r="C14" s="32" t="s">
+        <v>113</v>
+      </c>
+      <c r="D14" s="32" t="s">
+        <v>115</v>
+      </c>
+      <c r="E14" s="33" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="116" x14ac:dyDescent="0.35">
+      <c r="A15" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="B15" s="32" t="s">
+        <v>117</v>
+      </c>
+      <c r="C15" s="32" t="s">
+        <v>118</v>
+      </c>
+      <c r="D15" s="32" t="s">
+        <v>119</v>
+      </c>
+      <c r="E15" s="33" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A16" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B16" s="32" t="s">
+        <v>208</v>
+      </c>
+      <c r="C16" s="32" t="s">
+        <v>179</v>
+      </c>
+      <c r="D16" s="32" t="s">
+        <v>126</v>
+      </c>
+      <c r="E16" s="33" t="s">
         <v>110</v>
       </c>
-      <c r="D3" s="41" t="s">
-        <v>107</v>
-      </c>
-      <c r="E3" s="42" t="s">
+    </row>
+    <row r="17" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A17" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="B17" s="32" t="s">
+        <v>124</v>
+      </c>
+      <c r="C17" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="D17" s="32" t="s">
+        <v>126</v>
+      </c>
+      <c r="E17" s="33" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+      <c r="A18" s="5" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="36" t="s">
-        <v>113</v>
-      </c>
-      <c r="B4" s="43" t="s">
-        <v>108</v>
-      </c>
-      <c r="C4" s="43" t="s">
-        <v>111</v>
-      </c>
-      <c r="D4" s="44" t="s">
-        <v>2</v>
-      </c>
-      <c r="E4" s="48"/>
-    </row>
-    <row r="5" spans="1:5" ht="58" x14ac:dyDescent="0.35">
-      <c r="A5" s="36" t="s">
-        <v>115</v>
-      </c>
-      <c r="B5" s="43" t="s">
+      <c r="B18" s="32" t="s">
+        <v>133</v>
+      </c>
+      <c r="C18" s="32" t="s">
+        <v>136</v>
+      </c>
+      <c r="D18" s="32" t="s">
+        <v>138</v>
+      </c>
+      <c r="E18" s="33" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A19" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="B19" s="32" t="s">
+        <v>135</v>
+      </c>
+      <c r="C19" s="32" t="s">
+        <v>137</v>
+      </c>
+      <c r="D19" s="32" t="s">
+        <v>139</v>
+      </c>
+      <c r="E19" s="33" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A20" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="B20" s="32" t="s">
+        <v>184</v>
+      </c>
+      <c r="C20" s="32" t="s">
+        <v>186</v>
+      </c>
+      <c r="D20" s="32" t="s">
+        <v>139</v>
+      </c>
+      <c r="E20" s="33" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+      <c r="A21" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="B21" s="32" t="s">
+        <v>189</v>
+      </c>
+      <c r="C21" s="32" t="s">
+        <v>190</v>
+      </c>
+      <c r="D21" s="32" t="s">
+        <v>139</v>
+      </c>
+      <c r="E21" s="33"/>
+    </row>
+    <row r="22" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+      <c r="A22" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="B22" s="32" t="s">
+        <v>193</v>
+      </c>
+      <c r="C22" s="32" t="s">
+        <v>194</v>
+      </c>
+      <c r="D22" s="32" t="s">
+        <v>139</v>
+      </c>
+      <c r="E22" s="33" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+      <c r="A23" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="B23" s="32" t="s">
+        <v>200</v>
+      </c>
+      <c r="C23" s="32" t="s">
+        <v>201</v>
+      </c>
+      <c r="D23" s="32" t="s">
+        <v>139</v>
+      </c>
+      <c r="E23" s="33" t="s">
         <v>132</v>
       </c>
-      <c r="C5" s="43" t="s">
-        <v>130</v>
-      </c>
-      <c r="D5" s="44" t="s">
-        <v>133</v>
-      </c>
-      <c r="E5" s="45"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B6" s="44"/>
-      <c r="C6" s="44"/>
-      <c r="D6" s="44"/>
-      <c r="E6" s="45"/>
-    </row>
-    <row r="7" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="44"/>
-      <c r="C7" s="44"/>
-      <c r="D7" s="44"/>
-      <c r="E7" s="45"/>
-    </row>
-    <row r="8" spans="1:5" ht="24.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B8" s="37"/>
-      <c r="C8" s="38"/>
-      <c r="D8" s="38" t="s">
-        <v>79</v>
-      </c>
-      <c r="E8" s="39"/>
-    </row>
-    <row r="9" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="36" t="s">
-        <v>112</v>
-      </c>
-      <c r="B9" s="40" t="s">
-        <v>109</v>
-      </c>
-      <c r="C9" s="41" t="s">
+    </row>
+    <row r="24" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A24" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="B24" s="32" t="s">
+        <v>207</v>
+      </c>
+      <c r="C24" s="32" t="s">
+        <v>179</v>
+      </c>
+      <c r="D24" s="50" t="s">
+        <v>205</v>
+      </c>
+      <c r="E24" s="33" t="s">
         <v>110</v>
       </c>
-      <c r="D9" s="41" t="s">
-        <v>119</v>
-      </c>
-      <c r="E9" s="42" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="116" x14ac:dyDescent="0.35">
-      <c r="A10" s="36" t="s">
-        <v>116</v>
-      </c>
-      <c r="B10" s="43" t="s">
-        <v>117</v>
-      </c>
-      <c r="C10" s="43" t="s">
-        <v>118</v>
-      </c>
-      <c r="D10" s="44" t="s">
-        <v>120</v>
-      </c>
-      <c r="E10" s="45" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="116" x14ac:dyDescent="0.35">
-      <c r="A11" s="36" t="s">
-        <v>121</v>
-      </c>
-      <c r="B11" s="43" t="s">
-        <v>122</v>
-      </c>
-      <c r="C11" s="43" t="s">
-        <v>123</v>
-      </c>
-      <c r="D11" s="44" t="s">
-        <v>124</v>
-      </c>
-      <c r="E11" s="45" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="36" t="s">
-        <v>128</v>
-      </c>
-      <c r="B12" s="43" t="s">
-        <v>129</v>
-      </c>
-      <c r="C12" s="43" t="s">
-        <v>130</v>
-      </c>
-      <c r="D12" s="44" t="s">
-        <v>131</v>
-      </c>
-      <c r="E12" s="48" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="58" x14ac:dyDescent="0.35">
-      <c r="A13" s="36" t="s">
-        <v>138</v>
-      </c>
-      <c r="B13" s="43" t="s">
+    </row>
+    <row r="25" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A25" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="B25" s="32" t="s">
+        <v>204</v>
+      </c>
+      <c r="C25" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="D25" s="50" t="s">
+        <v>205</v>
+      </c>
+      <c r="E25" s="33" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+      <c r="A26" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="B26" s="32" t="s">
+        <v>213</v>
+      </c>
+      <c r="C26" s="32" t="s">
+        <v>214</v>
+      </c>
+      <c r="D26" s="32" t="s">
         <v>139</v>
       </c>
-      <c r="C13" s="44" t="s">
-        <v>142</v>
-      </c>
-      <c r="D13" s="44" t="s">
-        <v>144</v>
-      </c>
-      <c r="E13" s="48" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="36" t="s">
-        <v>140</v>
-      </c>
-      <c r="B14" s="43" t="s">
-        <v>141</v>
-      </c>
-      <c r="C14" s="43" t="s">
-        <v>143</v>
-      </c>
-      <c r="D14" s="44" t="s">
-        <v>145</v>
-      </c>
-      <c r="E14" s="48" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B15" s="44"/>
-      <c r="C15" s="44"/>
-      <c r="D15" s="44"/>
-      <c r="E15" s="45"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B16" s="44"/>
-      <c r="C16" s="44"/>
-      <c r="D16" s="44"/>
-      <c r="E16" s="45"/>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B17" s="44"/>
-      <c r="C17" s="44"/>
-      <c r="D17" s="44"/>
-      <c r="E17" s="45"/>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B18" s="44"/>
-      <c r="C18" s="44"/>
-      <c r="D18" s="44"/>
-      <c r="E18" s="45"/>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B19" s="44"/>
-      <c r="C19" s="44"/>
-      <c r="D19" s="44"/>
-      <c r="E19" s="45"/>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B20" s="44"/>
-      <c r="C20" s="44"/>
-      <c r="D20" s="44"/>
-      <c r="E20" s="45"/>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B21" s="44"/>
-      <c r="C21" s="44"/>
-      <c r="D21" s="44"/>
-      <c r="E21" s="45"/>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B22" s="44"/>
-      <c r="C22" s="44"/>
-      <c r="D22" s="44"/>
-      <c r="E22" s="45"/>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B23" s="44"/>
-      <c r="C23" s="44"/>
-      <c r="D23" s="44"/>
-      <c r="E23" s="45"/>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B24" s="44"/>
-      <c r="C24" s="44"/>
-      <c r="D24" s="44"/>
-      <c r="E24" s="45"/>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B25" s="44"/>
-      <c r="C25" s="44"/>
-      <c r="D25" s="44"/>
-      <c r="E25" s="45"/>
-    </row>
-    <row r="26" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B26" s="46"/>
-      <c r="C26" s="46"/>
-      <c r="D26" s="46"/>
-      <c r="E26" s="47"/>
+      <c r="E26" s="33" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B27" s="32"/>
+      <c r="C27" s="32"/>
+      <c r="D27" s="32"/>
+      <c r="E27" s="33"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B28" s="32"/>
+      <c r="C28" s="32"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="33"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B29" s="32"/>
+      <c r="C29" s="32"/>
+      <c r="D29" s="32"/>
+      <c r="E29" s="33"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B30" s="32"/>
+      <c r="C30" s="32"/>
+      <c r="D30" s="32"/>
+      <c r="E30" s="33"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B31" s="32"/>
+      <c r="C31" s="32"/>
+      <c r="D31" s="32"/>
+      <c r="E31" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2478,6 +2779,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010013BCB5C12746E54CA9BC03E8B376BF68" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1260ad29e906c937f60b96f5873c5d20">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8253af2a-fd0f-40a4-8001-231cdeab6c87" xmlns:ns3="6b2d526b-f179-4f8c-9fce-7a2c6e455f6f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3126a3f5c1ef07429df3b7fa0c370d29" ns2:_="" ns3:_="">
     <xsd:import namespace="8253af2a-fd0f-40a4-8001-231cdeab6c87"/>
@@ -2700,15 +3010,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -2716,6 +3017,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E493745-6716-486B-A434-7B84E98D619F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923E968D-8884-44EF-83F3-2736A60A93CE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2734,14 +3043,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E493745-6716-486B-A434-7B84E98D619F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{967337ED-9C59-49A1-9209-B4AF8C9B52A5}">
   <ds:schemaRefs>

</xml_diff>